<commit_message>
Mise a jour du 09/01/2026
</commit_message>
<xml_diff>
--- a/TARIFS CORIS RETRAITE.xlsx
+++ b/TARIFS CORIS RETRAITE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://corisinvestgroup-my.sharepoint.com/personal/akambire_coris-assurances_com/Documents/Documents/DG CAV RCI 2025/Informations produits/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CORIS\app_coris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{24B68DDB-E4FF-496F-B476-76CD97D0F3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{294DBF3C-05C5-4D8F-968B-58E283AB1BEB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90D6CC5-8D76-460F-AC68-4A5AD9F8A695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LECTURE DE LA PRIME" sheetId="143" r:id="rId1"/>
@@ -46,14 +46,6 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -101,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -112,6 +104,7 @@
     <numFmt numFmtId="170" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="171" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -373,13 +366,11 @@
     <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="17" fillId="3" borderId="2" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -398,7 +389,9 @@
     <xf numFmtId="3" fontId="12" fillId="0" borderId="4" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Euro" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -483,9 +476,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -523,9 +516,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,26 +551,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -610,26 +586,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -809,151 +768,151 @@
   <dimension ref="A1:BN51"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="7" width="9.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="22" width="9.33203125" customWidth="1"/>
-    <col min="258" max="258" width="18.44140625" customWidth="1"/>
-    <col min="259" max="278" width="9.33203125" customWidth="1"/>
-    <col min="514" max="514" width="18.44140625" customWidth="1"/>
-    <col min="515" max="534" width="9.33203125" customWidth="1"/>
-    <col min="770" max="770" width="18.44140625" customWidth="1"/>
-    <col min="771" max="790" width="9.33203125" customWidth="1"/>
-    <col min="1026" max="1026" width="18.44140625" customWidth="1"/>
-    <col min="1027" max="1046" width="9.33203125" customWidth="1"/>
-    <col min="1282" max="1282" width="18.44140625" customWidth="1"/>
-    <col min="1283" max="1302" width="9.33203125" customWidth="1"/>
-    <col min="1538" max="1538" width="18.44140625" customWidth="1"/>
-    <col min="1539" max="1558" width="9.33203125" customWidth="1"/>
-    <col min="1794" max="1794" width="18.44140625" customWidth="1"/>
-    <col min="1795" max="1814" width="9.33203125" customWidth="1"/>
-    <col min="2050" max="2050" width="18.44140625" customWidth="1"/>
-    <col min="2051" max="2070" width="9.33203125" customWidth="1"/>
-    <col min="2306" max="2306" width="18.44140625" customWidth="1"/>
-    <col min="2307" max="2326" width="9.33203125" customWidth="1"/>
-    <col min="2562" max="2562" width="18.44140625" customWidth="1"/>
-    <col min="2563" max="2582" width="9.33203125" customWidth="1"/>
-    <col min="2818" max="2818" width="18.44140625" customWidth="1"/>
-    <col min="2819" max="2838" width="9.33203125" customWidth="1"/>
-    <col min="3074" max="3074" width="18.44140625" customWidth="1"/>
-    <col min="3075" max="3094" width="9.33203125" customWidth="1"/>
-    <col min="3330" max="3330" width="18.44140625" customWidth="1"/>
-    <col min="3331" max="3350" width="9.33203125" customWidth="1"/>
-    <col min="3586" max="3586" width="18.44140625" customWidth="1"/>
-    <col min="3587" max="3606" width="9.33203125" customWidth="1"/>
-    <col min="3842" max="3842" width="18.44140625" customWidth="1"/>
-    <col min="3843" max="3862" width="9.33203125" customWidth="1"/>
-    <col min="4098" max="4098" width="18.44140625" customWidth="1"/>
-    <col min="4099" max="4118" width="9.33203125" customWidth="1"/>
-    <col min="4354" max="4354" width="18.44140625" customWidth="1"/>
-    <col min="4355" max="4374" width="9.33203125" customWidth="1"/>
-    <col min="4610" max="4610" width="18.44140625" customWidth="1"/>
-    <col min="4611" max="4630" width="9.33203125" customWidth="1"/>
-    <col min="4866" max="4866" width="18.44140625" customWidth="1"/>
-    <col min="4867" max="4886" width="9.33203125" customWidth="1"/>
-    <col min="5122" max="5122" width="18.44140625" customWidth="1"/>
-    <col min="5123" max="5142" width="9.33203125" customWidth="1"/>
-    <col min="5378" max="5378" width="18.44140625" customWidth="1"/>
-    <col min="5379" max="5398" width="9.33203125" customWidth="1"/>
-    <col min="5634" max="5634" width="18.44140625" customWidth="1"/>
-    <col min="5635" max="5654" width="9.33203125" customWidth="1"/>
-    <col min="5890" max="5890" width="18.44140625" customWidth="1"/>
-    <col min="5891" max="5910" width="9.33203125" customWidth="1"/>
-    <col min="6146" max="6146" width="18.44140625" customWidth="1"/>
-    <col min="6147" max="6166" width="9.33203125" customWidth="1"/>
-    <col min="6402" max="6402" width="18.44140625" customWidth="1"/>
-    <col min="6403" max="6422" width="9.33203125" customWidth="1"/>
-    <col min="6658" max="6658" width="18.44140625" customWidth="1"/>
-    <col min="6659" max="6678" width="9.33203125" customWidth="1"/>
-    <col min="6914" max="6914" width="18.44140625" customWidth="1"/>
-    <col min="6915" max="6934" width="9.33203125" customWidth="1"/>
-    <col min="7170" max="7170" width="18.44140625" customWidth="1"/>
-    <col min="7171" max="7190" width="9.33203125" customWidth="1"/>
-    <col min="7426" max="7426" width="18.44140625" customWidth="1"/>
-    <col min="7427" max="7446" width="9.33203125" customWidth="1"/>
-    <col min="7682" max="7682" width="18.44140625" customWidth="1"/>
-    <col min="7683" max="7702" width="9.33203125" customWidth="1"/>
-    <col min="7938" max="7938" width="18.44140625" customWidth="1"/>
-    <col min="7939" max="7958" width="9.33203125" customWidth="1"/>
-    <col min="8194" max="8194" width="18.44140625" customWidth="1"/>
-    <col min="8195" max="8214" width="9.33203125" customWidth="1"/>
-    <col min="8450" max="8450" width="18.44140625" customWidth="1"/>
-    <col min="8451" max="8470" width="9.33203125" customWidth="1"/>
-    <col min="8706" max="8706" width="18.44140625" customWidth="1"/>
-    <col min="8707" max="8726" width="9.33203125" customWidth="1"/>
-    <col min="8962" max="8962" width="18.44140625" customWidth="1"/>
-    <col min="8963" max="8982" width="9.33203125" customWidth="1"/>
-    <col min="9218" max="9218" width="18.44140625" customWidth="1"/>
-    <col min="9219" max="9238" width="9.33203125" customWidth="1"/>
-    <col min="9474" max="9474" width="18.44140625" customWidth="1"/>
-    <col min="9475" max="9494" width="9.33203125" customWidth="1"/>
-    <col min="9730" max="9730" width="18.44140625" customWidth="1"/>
-    <col min="9731" max="9750" width="9.33203125" customWidth="1"/>
-    <col min="9986" max="9986" width="18.44140625" customWidth="1"/>
-    <col min="9987" max="10006" width="9.33203125" customWidth="1"/>
-    <col min="10242" max="10242" width="18.44140625" customWidth="1"/>
-    <col min="10243" max="10262" width="9.33203125" customWidth="1"/>
-    <col min="10498" max="10498" width="18.44140625" customWidth="1"/>
-    <col min="10499" max="10518" width="9.33203125" customWidth="1"/>
-    <col min="10754" max="10754" width="18.44140625" customWidth="1"/>
-    <col min="10755" max="10774" width="9.33203125" customWidth="1"/>
-    <col min="11010" max="11010" width="18.44140625" customWidth="1"/>
-    <col min="11011" max="11030" width="9.33203125" customWidth="1"/>
-    <col min="11266" max="11266" width="18.44140625" customWidth="1"/>
-    <col min="11267" max="11286" width="9.33203125" customWidth="1"/>
-    <col min="11522" max="11522" width="18.44140625" customWidth="1"/>
-    <col min="11523" max="11542" width="9.33203125" customWidth="1"/>
-    <col min="11778" max="11778" width="18.44140625" customWidth="1"/>
-    <col min="11779" max="11798" width="9.33203125" customWidth="1"/>
-    <col min="12034" max="12034" width="18.44140625" customWidth="1"/>
-    <col min="12035" max="12054" width="9.33203125" customWidth="1"/>
-    <col min="12290" max="12290" width="18.44140625" customWidth="1"/>
-    <col min="12291" max="12310" width="9.33203125" customWidth="1"/>
-    <col min="12546" max="12546" width="18.44140625" customWidth="1"/>
-    <col min="12547" max="12566" width="9.33203125" customWidth="1"/>
-    <col min="12802" max="12802" width="18.44140625" customWidth="1"/>
-    <col min="12803" max="12822" width="9.33203125" customWidth="1"/>
-    <col min="13058" max="13058" width="18.44140625" customWidth="1"/>
-    <col min="13059" max="13078" width="9.33203125" customWidth="1"/>
-    <col min="13314" max="13314" width="18.44140625" customWidth="1"/>
-    <col min="13315" max="13334" width="9.33203125" customWidth="1"/>
-    <col min="13570" max="13570" width="18.44140625" customWidth="1"/>
-    <col min="13571" max="13590" width="9.33203125" customWidth="1"/>
-    <col min="13826" max="13826" width="18.44140625" customWidth="1"/>
-    <col min="13827" max="13846" width="9.33203125" customWidth="1"/>
-    <col min="14082" max="14082" width="18.44140625" customWidth="1"/>
-    <col min="14083" max="14102" width="9.33203125" customWidth="1"/>
-    <col min="14338" max="14338" width="18.44140625" customWidth="1"/>
-    <col min="14339" max="14358" width="9.33203125" customWidth="1"/>
-    <col min="14594" max="14594" width="18.44140625" customWidth="1"/>
-    <col min="14595" max="14614" width="9.33203125" customWidth="1"/>
-    <col min="14850" max="14850" width="18.44140625" customWidth="1"/>
-    <col min="14851" max="14870" width="9.33203125" customWidth="1"/>
-    <col min="15106" max="15106" width="18.44140625" customWidth="1"/>
-    <col min="15107" max="15126" width="9.33203125" customWidth="1"/>
-    <col min="15362" max="15362" width="18.44140625" customWidth="1"/>
-    <col min="15363" max="15382" width="9.33203125" customWidth="1"/>
-    <col min="15618" max="15618" width="18.44140625" customWidth="1"/>
-    <col min="15619" max="15638" width="9.33203125" customWidth="1"/>
-    <col min="15874" max="15874" width="18.44140625" customWidth="1"/>
-    <col min="15875" max="15894" width="9.33203125" customWidth="1"/>
-    <col min="16130" max="16130" width="18.44140625" customWidth="1"/>
-    <col min="16131" max="16150" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
+    <col min="5" max="5" width="24.6328125" customWidth="1"/>
+    <col min="6" max="7" width="9.36328125" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="22" width="9.36328125" customWidth="1"/>
+    <col min="258" max="258" width="18.453125" customWidth="1"/>
+    <col min="259" max="278" width="9.36328125" customWidth="1"/>
+    <col min="514" max="514" width="18.453125" customWidth="1"/>
+    <col min="515" max="534" width="9.36328125" customWidth="1"/>
+    <col min="770" max="770" width="18.453125" customWidth="1"/>
+    <col min="771" max="790" width="9.36328125" customWidth="1"/>
+    <col min="1026" max="1026" width="18.453125" customWidth="1"/>
+    <col min="1027" max="1046" width="9.36328125" customWidth="1"/>
+    <col min="1282" max="1282" width="18.453125" customWidth="1"/>
+    <col min="1283" max="1302" width="9.36328125" customWidth="1"/>
+    <col min="1538" max="1538" width="18.453125" customWidth="1"/>
+    <col min="1539" max="1558" width="9.36328125" customWidth="1"/>
+    <col min="1794" max="1794" width="18.453125" customWidth="1"/>
+    <col min="1795" max="1814" width="9.36328125" customWidth="1"/>
+    <col min="2050" max="2050" width="18.453125" customWidth="1"/>
+    <col min="2051" max="2070" width="9.36328125" customWidth="1"/>
+    <col min="2306" max="2306" width="18.453125" customWidth="1"/>
+    <col min="2307" max="2326" width="9.36328125" customWidth="1"/>
+    <col min="2562" max="2562" width="18.453125" customWidth="1"/>
+    <col min="2563" max="2582" width="9.36328125" customWidth="1"/>
+    <col min="2818" max="2818" width="18.453125" customWidth="1"/>
+    <col min="2819" max="2838" width="9.36328125" customWidth="1"/>
+    <col min="3074" max="3074" width="18.453125" customWidth="1"/>
+    <col min="3075" max="3094" width="9.36328125" customWidth="1"/>
+    <col min="3330" max="3330" width="18.453125" customWidth="1"/>
+    <col min="3331" max="3350" width="9.36328125" customWidth="1"/>
+    <col min="3586" max="3586" width="18.453125" customWidth="1"/>
+    <col min="3587" max="3606" width="9.36328125" customWidth="1"/>
+    <col min="3842" max="3842" width="18.453125" customWidth="1"/>
+    <col min="3843" max="3862" width="9.36328125" customWidth="1"/>
+    <col min="4098" max="4098" width="18.453125" customWidth="1"/>
+    <col min="4099" max="4118" width="9.36328125" customWidth="1"/>
+    <col min="4354" max="4354" width="18.453125" customWidth="1"/>
+    <col min="4355" max="4374" width="9.36328125" customWidth="1"/>
+    <col min="4610" max="4610" width="18.453125" customWidth="1"/>
+    <col min="4611" max="4630" width="9.36328125" customWidth="1"/>
+    <col min="4866" max="4866" width="18.453125" customWidth="1"/>
+    <col min="4867" max="4886" width="9.36328125" customWidth="1"/>
+    <col min="5122" max="5122" width="18.453125" customWidth="1"/>
+    <col min="5123" max="5142" width="9.36328125" customWidth="1"/>
+    <col min="5378" max="5378" width="18.453125" customWidth="1"/>
+    <col min="5379" max="5398" width="9.36328125" customWidth="1"/>
+    <col min="5634" max="5634" width="18.453125" customWidth="1"/>
+    <col min="5635" max="5654" width="9.36328125" customWidth="1"/>
+    <col min="5890" max="5890" width="18.453125" customWidth="1"/>
+    <col min="5891" max="5910" width="9.36328125" customWidth="1"/>
+    <col min="6146" max="6146" width="18.453125" customWidth="1"/>
+    <col min="6147" max="6166" width="9.36328125" customWidth="1"/>
+    <col min="6402" max="6402" width="18.453125" customWidth="1"/>
+    <col min="6403" max="6422" width="9.36328125" customWidth="1"/>
+    <col min="6658" max="6658" width="18.453125" customWidth="1"/>
+    <col min="6659" max="6678" width="9.36328125" customWidth="1"/>
+    <col min="6914" max="6914" width="18.453125" customWidth="1"/>
+    <col min="6915" max="6934" width="9.36328125" customWidth="1"/>
+    <col min="7170" max="7170" width="18.453125" customWidth="1"/>
+    <col min="7171" max="7190" width="9.36328125" customWidth="1"/>
+    <col min="7426" max="7426" width="18.453125" customWidth="1"/>
+    <col min="7427" max="7446" width="9.36328125" customWidth="1"/>
+    <col min="7682" max="7682" width="18.453125" customWidth="1"/>
+    <col min="7683" max="7702" width="9.36328125" customWidth="1"/>
+    <col min="7938" max="7938" width="18.453125" customWidth="1"/>
+    <col min="7939" max="7958" width="9.36328125" customWidth="1"/>
+    <col min="8194" max="8194" width="18.453125" customWidth="1"/>
+    <col min="8195" max="8214" width="9.36328125" customWidth="1"/>
+    <col min="8450" max="8450" width="18.453125" customWidth="1"/>
+    <col min="8451" max="8470" width="9.36328125" customWidth="1"/>
+    <col min="8706" max="8706" width="18.453125" customWidth="1"/>
+    <col min="8707" max="8726" width="9.36328125" customWidth="1"/>
+    <col min="8962" max="8962" width="18.453125" customWidth="1"/>
+    <col min="8963" max="8982" width="9.36328125" customWidth="1"/>
+    <col min="9218" max="9218" width="18.453125" customWidth="1"/>
+    <col min="9219" max="9238" width="9.36328125" customWidth="1"/>
+    <col min="9474" max="9474" width="18.453125" customWidth="1"/>
+    <col min="9475" max="9494" width="9.36328125" customWidth="1"/>
+    <col min="9730" max="9730" width="18.453125" customWidth="1"/>
+    <col min="9731" max="9750" width="9.36328125" customWidth="1"/>
+    <col min="9986" max="9986" width="18.453125" customWidth="1"/>
+    <col min="9987" max="10006" width="9.36328125" customWidth="1"/>
+    <col min="10242" max="10242" width="18.453125" customWidth="1"/>
+    <col min="10243" max="10262" width="9.36328125" customWidth="1"/>
+    <col min="10498" max="10498" width="18.453125" customWidth="1"/>
+    <col min="10499" max="10518" width="9.36328125" customWidth="1"/>
+    <col min="10754" max="10754" width="18.453125" customWidth="1"/>
+    <col min="10755" max="10774" width="9.36328125" customWidth="1"/>
+    <col min="11010" max="11010" width="18.453125" customWidth="1"/>
+    <col min="11011" max="11030" width="9.36328125" customWidth="1"/>
+    <col min="11266" max="11266" width="18.453125" customWidth="1"/>
+    <col min="11267" max="11286" width="9.36328125" customWidth="1"/>
+    <col min="11522" max="11522" width="18.453125" customWidth="1"/>
+    <col min="11523" max="11542" width="9.36328125" customWidth="1"/>
+    <col min="11778" max="11778" width="18.453125" customWidth="1"/>
+    <col min="11779" max="11798" width="9.36328125" customWidth="1"/>
+    <col min="12034" max="12034" width="18.453125" customWidth="1"/>
+    <col min="12035" max="12054" width="9.36328125" customWidth="1"/>
+    <col min="12290" max="12290" width="18.453125" customWidth="1"/>
+    <col min="12291" max="12310" width="9.36328125" customWidth="1"/>
+    <col min="12546" max="12546" width="18.453125" customWidth="1"/>
+    <col min="12547" max="12566" width="9.36328125" customWidth="1"/>
+    <col min="12802" max="12802" width="18.453125" customWidth="1"/>
+    <col min="12803" max="12822" width="9.36328125" customWidth="1"/>
+    <col min="13058" max="13058" width="18.453125" customWidth="1"/>
+    <col min="13059" max="13078" width="9.36328125" customWidth="1"/>
+    <col min="13314" max="13314" width="18.453125" customWidth="1"/>
+    <col min="13315" max="13334" width="9.36328125" customWidth="1"/>
+    <col min="13570" max="13570" width="18.453125" customWidth="1"/>
+    <col min="13571" max="13590" width="9.36328125" customWidth="1"/>
+    <col min="13826" max="13826" width="18.453125" customWidth="1"/>
+    <col min="13827" max="13846" width="9.36328125" customWidth="1"/>
+    <col min="14082" max="14082" width="18.453125" customWidth="1"/>
+    <col min="14083" max="14102" width="9.36328125" customWidth="1"/>
+    <col min="14338" max="14338" width="18.453125" customWidth="1"/>
+    <col min="14339" max="14358" width="9.36328125" customWidth="1"/>
+    <col min="14594" max="14594" width="18.453125" customWidth="1"/>
+    <col min="14595" max="14614" width="9.36328125" customWidth="1"/>
+    <col min="14850" max="14850" width="18.453125" customWidth="1"/>
+    <col min="14851" max="14870" width="9.36328125" customWidth="1"/>
+    <col min="15106" max="15106" width="18.453125" customWidth="1"/>
+    <col min="15107" max="15126" width="9.36328125" customWidth="1"/>
+    <col min="15362" max="15362" width="18.453125" customWidth="1"/>
+    <col min="15363" max="15382" width="9.36328125" customWidth="1"/>
+    <col min="15618" max="15618" width="18.453125" customWidth="1"/>
+    <col min="15619" max="15638" width="9.36328125" customWidth="1"/>
+    <col min="15874" max="15874" width="18.453125" customWidth="1"/>
+    <col min="15875" max="15894" width="9.36328125" customWidth="1"/>
+    <col min="16130" max="16130" width="18.453125" customWidth="1"/>
+    <col min="16131" max="16150" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="3" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" s="3" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
@@ -1021,7 +980,7 @@
       <c r="BM1" s="10"/>
       <c r="BN1" s="10"/>
     </row>
-    <row r="2" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1031,7 +990,7 @@
       <c r="AC2" s="4"/>
       <c r="AY2" s="4"/>
     </row>
-    <row r="3" spans="1:66" s="3" customFormat="1" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:66" s="3" customFormat="1" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1107,7 +1066,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="12">
         <v>5</v>
       </c>
@@ -1183,7 +1142,7 @@
       <c r="BM4" s="9"/>
       <c r="BN4" s="9"/>
     </row>
-    <row r="5" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12">
         <v>6</v>
       </c>
@@ -1259,7 +1218,7 @@
       <c r="BM5" s="9"/>
       <c r="BN5" s="9"/>
     </row>
-    <row r="6" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="12">
         <v>7</v>
       </c>
@@ -1277,7 +1236,7 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="24">
+      <c r="H6" s="17">
         <v>15000000</v>
       </c>
       <c r="I6" s="9"/>
@@ -1337,7 +1296,7 @@
       <c r="BM6" s="9"/>
       <c r="BN6" s="9"/>
     </row>
-    <row r="7" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="12">
         <v>8</v>
       </c>
@@ -1413,7 +1372,7 @@
       <c r="BM7" s="9"/>
       <c r="BN7" s="9"/>
     </row>
-    <row r="8" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="12">
         <v>9</v>
       </c>
@@ -1489,7 +1448,7 @@
       <c r="BM8" s="9"/>
       <c r="BN8" s="9"/>
     </row>
-    <row r="9" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="12">
         <v>10</v>
       </c>
@@ -1565,7 +1524,7 @@
       <c r="BM9" s="9"/>
       <c r="BN9" s="9"/>
     </row>
-    <row r="10" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="12">
         <v>11</v>
       </c>
@@ -1641,7 +1600,7 @@
       <c r="BM10" s="9"/>
       <c r="BN10" s="9"/>
     </row>
-    <row r="11" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="12">
         <v>12</v>
       </c>
@@ -1717,7 +1676,7 @@
       <c r="BM11" s="9"/>
       <c r="BN11" s="9"/>
     </row>
-    <row r="12" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="12">
         <v>13</v>
       </c>
@@ -1793,7 +1752,7 @@
       <c r="BM12" s="9"/>
       <c r="BN12" s="9"/>
     </row>
-    <row r="13" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="12">
         <v>14</v>
       </c>
@@ -1869,7 +1828,7 @@
       <c r="BM13" s="9"/>
       <c r="BN13" s="9"/>
     </row>
-    <row r="14" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="12">
         <v>15</v>
       </c>
@@ -1945,7 +1904,7 @@
       <c r="BM14" s="9"/>
       <c r="BN14" s="9"/>
     </row>
-    <row r="15" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="12">
         <v>16</v>
       </c>
@@ -2021,7 +1980,7 @@
       <c r="BM15" s="9"/>
       <c r="BN15" s="9"/>
     </row>
-    <row r="16" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="12">
         <v>17</v>
       </c>
@@ -2097,7 +2056,7 @@
       <c r="BM16" s="9"/>
       <c r="BN16" s="9"/>
     </row>
-    <row r="17" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="12">
         <v>18</v>
       </c>
@@ -2173,7 +2132,7 @@
       <c r="BM17" s="9"/>
       <c r="BN17" s="9"/>
     </row>
-    <row r="18" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="12">
         <v>19</v>
       </c>
@@ -2249,7 +2208,7 @@
       <c r="BM18" s="9"/>
       <c r="BN18" s="9"/>
     </row>
-    <row r="19" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="12">
         <v>20</v>
       </c>
@@ -2325,7 +2284,7 @@
       <c r="BM19" s="9"/>
       <c r="BN19" s="9"/>
     </row>
-    <row r="20" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="12">
         <v>21</v>
       </c>
@@ -2401,7 +2360,7 @@
       <c r="BM20" s="9"/>
       <c r="BN20" s="9"/>
     </row>
-    <row r="21" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="12">
         <v>22</v>
       </c>
@@ -2477,7 +2436,7 @@
       <c r="BM21" s="9"/>
       <c r="BN21" s="9"/>
     </row>
-    <row r="22" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="12">
         <v>23</v>
       </c>
@@ -2553,7 +2512,7 @@
       <c r="BM22" s="9"/>
       <c r="BN22" s="9"/>
     </row>
-    <row r="23" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="12">
         <v>24</v>
       </c>
@@ -2629,7 +2588,7 @@
       <c r="BM23" s="9"/>
       <c r="BN23" s="9"/>
     </row>
-    <row r="24" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="12">
         <v>25</v>
       </c>
@@ -2705,7 +2664,7 @@
       <c r="BM24" s="9"/>
       <c r="BN24" s="9"/>
     </row>
-    <row r="25" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="12">
         <v>26</v>
       </c>
@@ -2781,7 +2740,7 @@
       <c r="BM25" s="9"/>
       <c r="BN25" s="9"/>
     </row>
-    <row r="26" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="12">
         <v>27</v>
       </c>
@@ -2857,7 +2816,7 @@
       <c r="BM26" s="9"/>
       <c r="BN26" s="9"/>
     </row>
-    <row r="27" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="12">
         <v>28</v>
       </c>
@@ -2933,7 +2892,7 @@
       <c r="BM27" s="9"/>
       <c r="BN27" s="9"/>
     </row>
-    <row r="28" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="12">
         <v>29</v>
       </c>
@@ -3009,7 +2968,7 @@
       <c r="BM28" s="9"/>
       <c r="BN28" s="9"/>
     </row>
-    <row r="29" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="12">
         <v>30</v>
       </c>
@@ -3085,7 +3044,7 @@
       <c r="BM29" s="9"/>
       <c r="BN29" s="9"/>
     </row>
-    <row r="30" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="12">
         <v>31</v>
       </c>
@@ -3161,7 +3120,7 @@
       <c r="BM30" s="9"/>
       <c r="BN30" s="9"/>
     </row>
-    <row r="31" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="12">
         <v>32</v>
       </c>
@@ -3237,7 +3196,7 @@
       <c r="BM31" s="9"/>
       <c r="BN31" s="9"/>
     </row>
-    <row r="32" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="12">
         <v>33</v>
       </c>
@@ -3313,7 +3272,7 @@
       <c r="BM32" s="9"/>
       <c r="BN32" s="9"/>
     </row>
-    <row r="33" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="12">
         <v>34</v>
       </c>
@@ -3389,7 +3348,7 @@
       <c r="BM33" s="9"/>
       <c r="BN33" s="9"/>
     </row>
-    <row r="34" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="12">
         <v>35</v>
       </c>
@@ -3465,7 +3424,7 @@
       <c r="BM34" s="9"/>
       <c r="BN34" s="9"/>
     </row>
-    <row r="35" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="12">
         <v>36</v>
       </c>
@@ -3541,7 +3500,7 @@
       <c r="BM35" s="9"/>
       <c r="BN35" s="9"/>
     </row>
-    <row r="36" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="12">
         <v>37</v>
       </c>
@@ -3617,7 +3576,7 @@
       <c r="BM36" s="9"/>
       <c r="BN36" s="9"/>
     </row>
-    <row r="37" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="12">
         <v>38</v>
       </c>
@@ -3693,7 +3652,7 @@
       <c r="BM37" s="9"/>
       <c r="BN37" s="9"/>
     </row>
-    <row r="38" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="12">
         <v>39</v>
       </c>
@@ -3769,7 +3728,7 @@
       <c r="BM38" s="9"/>
       <c r="BN38" s="9"/>
     </row>
-    <row r="39" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="12">
         <v>40</v>
       </c>
@@ -3845,7 +3804,7 @@
       <c r="BM39" s="9"/>
       <c r="BN39" s="9"/>
     </row>
-    <row r="40" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="12">
         <v>41</v>
       </c>
@@ -3921,7 +3880,7 @@
       <c r="BM40" s="9"/>
       <c r="BN40" s="9"/>
     </row>
-    <row r="41" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="12">
         <v>42</v>
       </c>
@@ -3997,7 +3956,7 @@
       <c r="BM41" s="9"/>
       <c r="BN41" s="9"/>
     </row>
-    <row r="42" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="12">
         <v>43</v>
       </c>
@@ -4073,7 +4032,7 @@
       <c r="BM42" s="9"/>
       <c r="BN42" s="9"/>
     </row>
-    <row r="43" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="12">
         <v>44</v>
       </c>
@@ -4149,7 +4108,7 @@
       <c r="BM43" s="9"/>
       <c r="BN43" s="9"/>
     </row>
-    <row r="44" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="12">
         <v>45</v>
       </c>
@@ -4225,7 +4184,7 @@
       <c r="BM44" s="9"/>
       <c r="BN44" s="9"/>
     </row>
-    <row r="45" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="12">
         <v>46</v>
       </c>
@@ -4301,7 +4260,7 @@
       <c r="BM45" s="9"/>
       <c r="BN45" s="9"/>
     </row>
-    <row r="46" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="12">
         <v>47</v>
       </c>
@@ -4377,7 +4336,7 @@
       <c r="BM46" s="9"/>
       <c r="BN46" s="9"/>
     </row>
-    <row r="47" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="12">
         <v>48</v>
       </c>
@@ -4453,7 +4412,7 @@
       <c r="BM47" s="9"/>
       <c r="BN47" s="9"/>
     </row>
-    <row r="48" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="12">
         <v>49</v>
       </c>
@@ -4529,7 +4488,7 @@
       <c r="BM48" s="9"/>
       <c r="BN48" s="9"/>
     </row>
-    <row r="49" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="12">
         <v>50</v>
       </c>
@@ -4605,7 +4564,7 @@
       <c r="BM49" s="9"/>
       <c r="BN49" s="9"/>
     </row>
-    <row r="50" spans="1:66" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:66" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
@@ -4670,7 +4629,7 @@
       <c r="BM50" s="9"/>
       <c r="BN50" s="9"/>
     </row>
-    <row r="51" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:66" x14ac:dyDescent="0.35">
       <c r="B51" s="8"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
@@ -4762,149 +4721,149 @@
   </sheetPr>
   <dimension ref="A1:BN51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="22" width="9.33203125" customWidth="1"/>
-    <col min="258" max="258" width="18.44140625" customWidth="1"/>
-    <col min="259" max="278" width="9.33203125" customWidth="1"/>
-    <col min="514" max="514" width="18.44140625" customWidth="1"/>
-    <col min="515" max="534" width="9.33203125" customWidth="1"/>
-    <col min="770" max="770" width="18.44140625" customWidth="1"/>
-    <col min="771" max="790" width="9.33203125" customWidth="1"/>
-    <col min="1026" max="1026" width="18.44140625" customWidth="1"/>
-    <col min="1027" max="1046" width="9.33203125" customWidth="1"/>
-    <col min="1282" max="1282" width="18.44140625" customWidth="1"/>
-    <col min="1283" max="1302" width="9.33203125" customWidth="1"/>
-    <col min="1538" max="1538" width="18.44140625" customWidth="1"/>
-    <col min="1539" max="1558" width="9.33203125" customWidth="1"/>
-    <col min="1794" max="1794" width="18.44140625" customWidth="1"/>
-    <col min="1795" max="1814" width="9.33203125" customWidth="1"/>
-    <col min="2050" max="2050" width="18.44140625" customWidth="1"/>
-    <col min="2051" max="2070" width="9.33203125" customWidth="1"/>
-    <col min="2306" max="2306" width="18.44140625" customWidth="1"/>
-    <col min="2307" max="2326" width="9.33203125" customWidth="1"/>
-    <col min="2562" max="2562" width="18.44140625" customWidth="1"/>
-    <col min="2563" max="2582" width="9.33203125" customWidth="1"/>
-    <col min="2818" max="2818" width="18.44140625" customWidth="1"/>
-    <col min="2819" max="2838" width="9.33203125" customWidth="1"/>
-    <col min="3074" max="3074" width="18.44140625" customWidth="1"/>
-    <col min="3075" max="3094" width="9.33203125" customWidth="1"/>
-    <col min="3330" max="3330" width="18.44140625" customWidth="1"/>
-    <col min="3331" max="3350" width="9.33203125" customWidth="1"/>
-    <col min="3586" max="3586" width="18.44140625" customWidth="1"/>
-    <col min="3587" max="3606" width="9.33203125" customWidth="1"/>
-    <col min="3842" max="3842" width="18.44140625" customWidth="1"/>
-    <col min="3843" max="3862" width="9.33203125" customWidth="1"/>
-    <col min="4098" max="4098" width="18.44140625" customWidth="1"/>
-    <col min="4099" max="4118" width="9.33203125" customWidth="1"/>
-    <col min="4354" max="4354" width="18.44140625" customWidth="1"/>
-    <col min="4355" max="4374" width="9.33203125" customWidth="1"/>
-    <col min="4610" max="4610" width="18.44140625" customWidth="1"/>
-    <col min="4611" max="4630" width="9.33203125" customWidth="1"/>
-    <col min="4866" max="4866" width="18.44140625" customWidth="1"/>
-    <col min="4867" max="4886" width="9.33203125" customWidth="1"/>
-    <col min="5122" max="5122" width="18.44140625" customWidth="1"/>
-    <col min="5123" max="5142" width="9.33203125" customWidth="1"/>
-    <col min="5378" max="5378" width="18.44140625" customWidth="1"/>
-    <col min="5379" max="5398" width="9.33203125" customWidth="1"/>
-    <col min="5634" max="5634" width="18.44140625" customWidth="1"/>
-    <col min="5635" max="5654" width="9.33203125" customWidth="1"/>
-    <col min="5890" max="5890" width="18.44140625" customWidth="1"/>
-    <col min="5891" max="5910" width="9.33203125" customWidth="1"/>
-    <col min="6146" max="6146" width="18.44140625" customWidth="1"/>
-    <col min="6147" max="6166" width="9.33203125" customWidth="1"/>
-    <col min="6402" max="6402" width="18.44140625" customWidth="1"/>
-    <col min="6403" max="6422" width="9.33203125" customWidth="1"/>
-    <col min="6658" max="6658" width="18.44140625" customWidth="1"/>
-    <col min="6659" max="6678" width="9.33203125" customWidth="1"/>
-    <col min="6914" max="6914" width="18.44140625" customWidth="1"/>
-    <col min="6915" max="6934" width="9.33203125" customWidth="1"/>
-    <col min="7170" max="7170" width="18.44140625" customWidth="1"/>
-    <col min="7171" max="7190" width="9.33203125" customWidth="1"/>
-    <col min="7426" max="7426" width="18.44140625" customWidth="1"/>
-    <col min="7427" max="7446" width="9.33203125" customWidth="1"/>
-    <col min="7682" max="7682" width="18.44140625" customWidth="1"/>
-    <col min="7683" max="7702" width="9.33203125" customWidth="1"/>
-    <col min="7938" max="7938" width="18.44140625" customWidth="1"/>
-    <col min="7939" max="7958" width="9.33203125" customWidth="1"/>
-    <col min="8194" max="8194" width="18.44140625" customWidth="1"/>
-    <col min="8195" max="8214" width="9.33203125" customWidth="1"/>
-    <col min="8450" max="8450" width="18.44140625" customWidth="1"/>
-    <col min="8451" max="8470" width="9.33203125" customWidth="1"/>
-    <col min="8706" max="8706" width="18.44140625" customWidth="1"/>
-    <col min="8707" max="8726" width="9.33203125" customWidth="1"/>
-    <col min="8962" max="8962" width="18.44140625" customWidth="1"/>
-    <col min="8963" max="8982" width="9.33203125" customWidth="1"/>
-    <col min="9218" max="9218" width="18.44140625" customWidth="1"/>
-    <col min="9219" max="9238" width="9.33203125" customWidth="1"/>
-    <col min="9474" max="9474" width="18.44140625" customWidth="1"/>
-    <col min="9475" max="9494" width="9.33203125" customWidth="1"/>
-    <col min="9730" max="9730" width="18.44140625" customWidth="1"/>
-    <col min="9731" max="9750" width="9.33203125" customWidth="1"/>
-    <col min="9986" max="9986" width="18.44140625" customWidth="1"/>
-    <col min="9987" max="10006" width="9.33203125" customWidth="1"/>
-    <col min="10242" max="10242" width="18.44140625" customWidth="1"/>
-    <col min="10243" max="10262" width="9.33203125" customWidth="1"/>
-    <col min="10498" max="10498" width="18.44140625" customWidth="1"/>
-    <col min="10499" max="10518" width="9.33203125" customWidth="1"/>
-    <col min="10754" max="10754" width="18.44140625" customWidth="1"/>
-    <col min="10755" max="10774" width="9.33203125" customWidth="1"/>
-    <col min="11010" max="11010" width="18.44140625" customWidth="1"/>
-    <col min="11011" max="11030" width="9.33203125" customWidth="1"/>
-    <col min="11266" max="11266" width="18.44140625" customWidth="1"/>
-    <col min="11267" max="11286" width="9.33203125" customWidth="1"/>
-    <col min="11522" max="11522" width="18.44140625" customWidth="1"/>
-    <col min="11523" max="11542" width="9.33203125" customWidth="1"/>
-    <col min="11778" max="11778" width="18.44140625" customWidth="1"/>
-    <col min="11779" max="11798" width="9.33203125" customWidth="1"/>
-    <col min="12034" max="12034" width="18.44140625" customWidth="1"/>
-    <col min="12035" max="12054" width="9.33203125" customWidth="1"/>
-    <col min="12290" max="12290" width="18.44140625" customWidth="1"/>
-    <col min="12291" max="12310" width="9.33203125" customWidth="1"/>
-    <col min="12546" max="12546" width="18.44140625" customWidth="1"/>
-    <col min="12547" max="12566" width="9.33203125" customWidth="1"/>
-    <col min="12802" max="12802" width="18.44140625" customWidth="1"/>
-    <col min="12803" max="12822" width="9.33203125" customWidth="1"/>
-    <col min="13058" max="13058" width="18.44140625" customWidth="1"/>
-    <col min="13059" max="13078" width="9.33203125" customWidth="1"/>
-    <col min="13314" max="13314" width="18.44140625" customWidth="1"/>
-    <col min="13315" max="13334" width="9.33203125" customWidth="1"/>
-    <col min="13570" max="13570" width="18.44140625" customWidth="1"/>
-    <col min="13571" max="13590" width="9.33203125" customWidth="1"/>
-    <col min="13826" max="13826" width="18.44140625" customWidth="1"/>
-    <col min="13827" max="13846" width="9.33203125" customWidth="1"/>
-    <col min="14082" max="14082" width="18.44140625" customWidth="1"/>
-    <col min="14083" max="14102" width="9.33203125" customWidth="1"/>
-    <col min="14338" max="14338" width="18.44140625" customWidth="1"/>
-    <col min="14339" max="14358" width="9.33203125" customWidth="1"/>
-    <col min="14594" max="14594" width="18.44140625" customWidth="1"/>
-    <col min="14595" max="14614" width="9.33203125" customWidth="1"/>
-    <col min="14850" max="14850" width="18.44140625" customWidth="1"/>
-    <col min="14851" max="14870" width="9.33203125" customWidth="1"/>
-    <col min="15106" max="15106" width="18.44140625" customWidth="1"/>
-    <col min="15107" max="15126" width="9.33203125" customWidth="1"/>
-    <col min="15362" max="15362" width="18.44140625" customWidth="1"/>
-    <col min="15363" max="15382" width="9.33203125" customWidth="1"/>
-    <col min="15618" max="15618" width="18.44140625" customWidth="1"/>
-    <col min="15619" max="15638" width="9.33203125" customWidth="1"/>
-    <col min="15874" max="15874" width="18.44140625" customWidth="1"/>
-    <col min="15875" max="15894" width="9.33203125" customWidth="1"/>
-    <col min="16130" max="16130" width="18.44140625" customWidth="1"/>
-    <col min="16131" max="16150" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="22" width="9.36328125" customWidth="1"/>
+    <col min="258" max="258" width="18.453125" customWidth="1"/>
+    <col min="259" max="278" width="9.36328125" customWidth="1"/>
+    <col min="514" max="514" width="18.453125" customWidth="1"/>
+    <col min="515" max="534" width="9.36328125" customWidth="1"/>
+    <col min="770" max="770" width="18.453125" customWidth="1"/>
+    <col min="771" max="790" width="9.36328125" customWidth="1"/>
+    <col min="1026" max="1026" width="18.453125" customWidth="1"/>
+    <col min="1027" max="1046" width="9.36328125" customWidth="1"/>
+    <col min="1282" max="1282" width="18.453125" customWidth="1"/>
+    <col min="1283" max="1302" width="9.36328125" customWidth="1"/>
+    <col min="1538" max="1538" width="18.453125" customWidth="1"/>
+    <col min="1539" max="1558" width="9.36328125" customWidth="1"/>
+    <col min="1794" max="1794" width="18.453125" customWidth="1"/>
+    <col min="1795" max="1814" width="9.36328125" customWidth="1"/>
+    <col min="2050" max="2050" width="18.453125" customWidth="1"/>
+    <col min="2051" max="2070" width="9.36328125" customWidth="1"/>
+    <col min="2306" max="2306" width="18.453125" customWidth="1"/>
+    <col min="2307" max="2326" width="9.36328125" customWidth="1"/>
+    <col min="2562" max="2562" width="18.453125" customWidth="1"/>
+    <col min="2563" max="2582" width="9.36328125" customWidth="1"/>
+    <col min="2818" max="2818" width="18.453125" customWidth="1"/>
+    <col min="2819" max="2838" width="9.36328125" customWidth="1"/>
+    <col min="3074" max="3074" width="18.453125" customWidth="1"/>
+    <col min="3075" max="3094" width="9.36328125" customWidth="1"/>
+    <col min="3330" max="3330" width="18.453125" customWidth="1"/>
+    <col min="3331" max="3350" width="9.36328125" customWidth="1"/>
+    <col min="3586" max="3586" width="18.453125" customWidth="1"/>
+    <col min="3587" max="3606" width="9.36328125" customWidth="1"/>
+    <col min="3842" max="3842" width="18.453125" customWidth="1"/>
+    <col min="3843" max="3862" width="9.36328125" customWidth="1"/>
+    <col min="4098" max="4098" width="18.453125" customWidth="1"/>
+    <col min="4099" max="4118" width="9.36328125" customWidth="1"/>
+    <col min="4354" max="4354" width="18.453125" customWidth="1"/>
+    <col min="4355" max="4374" width="9.36328125" customWidth="1"/>
+    <col min="4610" max="4610" width="18.453125" customWidth="1"/>
+    <col min="4611" max="4630" width="9.36328125" customWidth="1"/>
+    <col min="4866" max="4866" width="18.453125" customWidth="1"/>
+    <col min="4867" max="4886" width="9.36328125" customWidth="1"/>
+    <col min="5122" max="5122" width="18.453125" customWidth="1"/>
+    <col min="5123" max="5142" width="9.36328125" customWidth="1"/>
+    <col min="5378" max="5378" width="18.453125" customWidth="1"/>
+    <col min="5379" max="5398" width="9.36328125" customWidth="1"/>
+    <col min="5634" max="5634" width="18.453125" customWidth="1"/>
+    <col min="5635" max="5654" width="9.36328125" customWidth="1"/>
+    <col min="5890" max="5890" width="18.453125" customWidth="1"/>
+    <col min="5891" max="5910" width="9.36328125" customWidth="1"/>
+    <col min="6146" max="6146" width="18.453125" customWidth="1"/>
+    <col min="6147" max="6166" width="9.36328125" customWidth="1"/>
+    <col min="6402" max="6402" width="18.453125" customWidth="1"/>
+    <col min="6403" max="6422" width="9.36328125" customWidth="1"/>
+    <col min="6658" max="6658" width="18.453125" customWidth="1"/>
+    <col min="6659" max="6678" width="9.36328125" customWidth="1"/>
+    <col min="6914" max="6914" width="18.453125" customWidth="1"/>
+    <col min="6915" max="6934" width="9.36328125" customWidth="1"/>
+    <col min="7170" max="7170" width="18.453125" customWidth="1"/>
+    <col min="7171" max="7190" width="9.36328125" customWidth="1"/>
+    <col min="7426" max="7426" width="18.453125" customWidth="1"/>
+    <col min="7427" max="7446" width="9.36328125" customWidth="1"/>
+    <col min="7682" max="7682" width="18.453125" customWidth="1"/>
+    <col min="7683" max="7702" width="9.36328125" customWidth="1"/>
+    <col min="7938" max="7938" width="18.453125" customWidth="1"/>
+    <col min="7939" max="7958" width="9.36328125" customWidth="1"/>
+    <col min="8194" max="8194" width="18.453125" customWidth="1"/>
+    <col min="8195" max="8214" width="9.36328125" customWidth="1"/>
+    <col min="8450" max="8450" width="18.453125" customWidth="1"/>
+    <col min="8451" max="8470" width="9.36328125" customWidth="1"/>
+    <col min="8706" max="8706" width="18.453125" customWidth="1"/>
+    <col min="8707" max="8726" width="9.36328125" customWidth="1"/>
+    <col min="8962" max="8962" width="18.453125" customWidth="1"/>
+    <col min="8963" max="8982" width="9.36328125" customWidth="1"/>
+    <col min="9218" max="9218" width="18.453125" customWidth="1"/>
+    <col min="9219" max="9238" width="9.36328125" customWidth="1"/>
+    <col min="9474" max="9474" width="18.453125" customWidth="1"/>
+    <col min="9475" max="9494" width="9.36328125" customWidth="1"/>
+    <col min="9730" max="9730" width="18.453125" customWidth="1"/>
+    <col min="9731" max="9750" width="9.36328125" customWidth="1"/>
+    <col min="9986" max="9986" width="18.453125" customWidth="1"/>
+    <col min="9987" max="10006" width="9.36328125" customWidth="1"/>
+    <col min="10242" max="10242" width="18.453125" customWidth="1"/>
+    <col min="10243" max="10262" width="9.36328125" customWidth="1"/>
+    <col min="10498" max="10498" width="18.453125" customWidth="1"/>
+    <col min="10499" max="10518" width="9.36328125" customWidth="1"/>
+    <col min="10754" max="10754" width="18.453125" customWidth="1"/>
+    <col min="10755" max="10774" width="9.36328125" customWidth="1"/>
+    <col min="11010" max="11010" width="18.453125" customWidth="1"/>
+    <col min="11011" max="11030" width="9.36328125" customWidth="1"/>
+    <col min="11266" max="11266" width="18.453125" customWidth="1"/>
+    <col min="11267" max="11286" width="9.36328125" customWidth="1"/>
+    <col min="11522" max="11522" width="18.453125" customWidth="1"/>
+    <col min="11523" max="11542" width="9.36328125" customWidth="1"/>
+    <col min="11778" max="11778" width="18.453125" customWidth="1"/>
+    <col min="11779" max="11798" width="9.36328125" customWidth="1"/>
+    <col min="12034" max="12034" width="18.453125" customWidth="1"/>
+    <col min="12035" max="12054" width="9.36328125" customWidth="1"/>
+    <col min="12290" max="12290" width="18.453125" customWidth="1"/>
+    <col min="12291" max="12310" width="9.36328125" customWidth="1"/>
+    <col min="12546" max="12546" width="18.453125" customWidth="1"/>
+    <col min="12547" max="12566" width="9.36328125" customWidth="1"/>
+    <col min="12802" max="12802" width="18.453125" customWidth="1"/>
+    <col min="12803" max="12822" width="9.36328125" customWidth="1"/>
+    <col min="13058" max="13058" width="18.453125" customWidth="1"/>
+    <col min="13059" max="13078" width="9.36328125" customWidth="1"/>
+    <col min="13314" max="13314" width="18.453125" customWidth="1"/>
+    <col min="13315" max="13334" width="9.36328125" customWidth="1"/>
+    <col min="13570" max="13570" width="18.453125" customWidth="1"/>
+    <col min="13571" max="13590" width="9.36328125" customWidth="1"/>
+    <col min="13826" max="13826" width="18.453125" customWidth="1"/>
+    <col min="13827" max="13846" width="9.36328125" customWidth="1"/>
+    <col min="14082" max="14082" width="18.453125" customWidth="1"/>
+    <col min="14083" max="14102" width="9.36328125" customWidth="1"/>
+    <col min="14338" max="14338" width="18.453125" customWidth="1"/>
+    <col min="14339" max="14358" width="9.36328125" customWidth="1"/>
+    <col min="14594" max="14594" width="18.453125" customWidth="1"/>
+    <col min="14595" max="14614" width="9.36328125" customWidth="1"/>
+    <col min="14850" max="14850" width="18.453125" customWidth="1"/>
+    <col min="14851" max="14870" width="9.36328125" customWidth="1"/>
+    <col min="15106" max="15106" width="18.453125" customWidth="1"/>
+    <col min="15107" max="15126" width="9.36328125" customWidth="1"/>
+    <col min="15362" max="15362" width="18.453125" customWidth="1"/>
+    <col min="15363" max="15382" width="9.36328125" customWidth="1"/>
+    <col min="15618" max="15618" width="18.453125" customWidth="1"/>
+    <col min="15619" max="15638" width="9.36328125" customWidth="1"/>
+    <col min="15874" max="15874" width="18.453125" customWidth="1"/>
+    <col min="15875" max="15894" width="9.36328125" customWidth="1"/>
+    <col min="16130" max="16130" width="18.453125" customWidth="1"/>
+    <col min="16131" max="16150" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="3" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" s="3" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
         <v>9</v>
       </c>
@@ -4972,7 +4931,7 @@
       <c r="BM1" s="10"/>
       <c r="BN1" s="10"/>
     </row>
-    <row r="2" spans="1:66" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:66" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -4982,7 +4941,7 @@
       <c r="AC2" s="4"/>
       <c r="AY2" s="4"/>
     </row>
-    <row r="3" spans="1:66" s="3" customFormat="1" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:66" s="3" customFormat="1" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -5060,20 +5019,20 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16">
+    <row r="4" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="15">
         <v>5</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="24">
         <v>605463.4053790709</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="24">
         <v>615056.50412301975</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="24">
         <v>620331.44792828942</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="24">
         <v>625666.38810555974</v>
       </c>
       <c r="F4" s="9"/>
@@ -5136,20 +5095,20 @@
       <c r="BM4" s="9"/>
       <c r="BN4" s="9"/>
     </row>
-    <row r="5" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16">
+    <row r="5" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15">
         <v>6</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="24">
         <v>739294.36457714031</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="24">
         <v>752256.79522809363</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="24">
         <v>758213.77487759781</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="24">
         <v>764734.52301000908</v>
       </c>
       <c r="F5" s="9"/>
@@ -5212,24 +5171,24 @@
       <c r="BM5" s="9"/>
       <c r="BN5" s="9"/>
     </row>
-    <row r="6" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16">
+    <row r="6" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="15">
         <v>7</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="24">
         <v>877714.81096697133</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="24">
         <v>891453.7231989851</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="24">
         <v>898104.54641603201</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="24">
         <v>908670.04263611406</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -5288,20 +5247,20 @@
       <c r="BM6" s="9"/>
       <c r="BN6" s="9"/>
     </row>
-    <row r="7" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16">
+    <row r="7" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="15">
         <v>8</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="24">
         <v>1020882.0657269702</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="24">
         <v>1038327.916971718</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="24">
         <v>1045708.9318124113</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="24">
         <v>1057643.3054491328</v>
       </c>
       <c r="F7" s="9"/>
@@ -5364,20 +5323,20 @@
       <c r="BM7" s="9"/>
       <c r="BN7" s="9"/>
     </row>
-    <row r="8" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16">
+    <row r="8" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="15">
         <v>9</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="24">
         <v>1168958.8403962203</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="24">
         <v>1190342.7075264968</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="24">
         <v>1198479.4706976637</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="24">
         <v>1211830.632460607</v>
       </c>
       <c r="F8" s="9"/>
@@ -5440,20 +5399,20 @@
       <c r="BM8" s="9"/>
       <c r="BN8" s="9"/>
     </row>
-    <row r="9" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16">
+    <row r="9" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="15">
         <v>10</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="24">
         <v>1322113.4214812894</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="24">
         <v>1344567.6482015899</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="24">
         <v>1356596.9784439001</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="24">
         <v>1371414.515917483</v>
       </c>
       <c r="F9" s="9"/>
@@ -5516,20 +5475,20 @@
       <c r="BM9" s="9"/>
       <c r="BN9" s="9"/>
     </row>
-    <row r="10" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16">
+    <row r="10" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="15">
         <v>11</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="24">
         <v>1480519.8613823166</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="24">
         <v>1507300.829349414</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="24">
         <v>1520248.5989612546</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="24">
         <v>1536583.8352953496</v>
       </c>
       <c r="F10" s="9"/>
@@ -5592,20 +5551,20 @@
       <c r="BM10" s="9"/>
       <c r="BN10" s="9"/>
     </row>
-    <row r="11" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="16">
+    <row r="11" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="15">
         <v>12</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="24">
         <v>1644358.1758545868</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="24">
         <v>1675729.6718374125</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="24">
         <v>1689628.0261967166</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="24">
         <v>1707534.0808514415</v>
       </c>
       <c r="F11" s="9"/>
@@ -5668,20 +5627,20 @@
       <c r="BM11" s="9"/>
       <c r="BN11" s="9"/>
     </row>
-    <row r="12" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16">
+    <row r="12" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="15">
         <v>13</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="24">
         <v>1813814.5482292068</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="24">
         <v>1846605.0037129808</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="24">
         <v>1861472.3841258783</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="24">
         <v>1880974.4504378813</v>
       </c>
       <c r="F12" s="9"/>
@@ -5744,20 +5703,20 @@
       <c r="BM12" s="9"/>
       <c r="BN12" s="9"/>
     </row>
-    <row r="13" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16">
+    <row r="13" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="15">
         <v>14</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="24">
         <v>1989081.5406241165</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="24">
         <v>2026909.4923037037</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="24">
         <v>2042794.6438421025</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="24">
         <v>2063978.3675239617</v>
       </c>
       <c r="F13" s="9"/>
@@ -5820,20 +5779,20 @@
       <c r="BM13" s="9"/>
       <c r="BN13" s="9"/>
     </row>
-    <row r="14" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16">
+    <row r="14" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="15">
         <v>15</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="24">
         <v>2170358.312384577</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="24">
         <v>2213524.6379951015</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="24">
         <v>2230463.1826483947</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="24">
         <v>2253387.4217080544</v>
       </c>
       <c r="F14" s="9"/>
@@ -5896,20 +5855,20 @@
       <c r="BM14" s="9"/>
       <c r="BN14" s="9"/>
     </row>
-    <row r="15" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16">
+    <row r="15" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="15">
         <v>16</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="24">
         <v>2361663.3470470016</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="24">
         <v>2402847.8779090727</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="24">
         <v>2424700.1203129073</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="24">
         <v>2449425.7927885908</v>
       </c>
       <c r="F15" s="9"/>
@@ -5972,20 +5931,20 @@
       <c r="BM15" s="9"/>
       <c r="BN15" s="9"/>
     </row>
-    <row r="16" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="16">
+    <row r="16" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="15">
         <v>17</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="24">
         <v>2559664.0579226101</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="24">
         <v>2602620.8670966583</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="24">
         <v>2625735.3507956774</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="24">
         <v>2652325.5068569463</v>
       </c>
       <c r="F16" s="9"/>
@@ -6048,20 +6007,20 @@
       <c r="BM16" s="9"/>
       <c r="BN16" s="9"/>
     </row>
-    <row r="17" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16">
+    <row r="17" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="15">
         <v>18</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="24">
         <v>2764594.7936788616</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="24">
         <v>2809385.9109058101</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="24">
         <v>2833806.8143453449</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="24">
         <v>2862326.7109176936</v>
       </c>
       <c r="F17" s="9"/>
@@ -6124,20 +6083,20 @@
       <c r="BM17" s="9"/>
       <c r="BN17" s="9"/>
     </row>
-    <row r="18" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="16">
+    <row r="18" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="15">
         <v>19</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="24">
         <v>2976698.105186583</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="24">
         <v>3019148.6195479506</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="24">
         <v>3044903.4385949676</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="24">
         <v>3079677.9571205671</v>
       </c>
       <c r="F18" s="9"/>
@@ -6200,20 +6159,20 @@
       <c r="BM18" s="9"/>
       <c r="BN18" s="9"/>
     </row>
-    <row r="19" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="16">
+    <row r="19" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="15">
         <v>20</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="24">
         <v>3196225.0325970734</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="24">
         <v>3240492.1346928971</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="24">
         <v>3267645.7852176097</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="24">
         <v>3304636.4969405411</v>
       </c>
       <c r="F19" s="9"/>
@@ -6276,20 +6235,20 @@
       <c r="BM19" s="9"/>
       <c r="BN19" s="9"/>
     </row>
-    <row r="20" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16">
+    <row r="20" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="15">
         <v>21</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="24">
         <v>3423435.4024669314</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="24">
         <v>3469582.6728679161</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="24">
         <v>3498184.1139720445</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="24">
         <v>3537468.5856542145</v>
       </c>
       <c r="F20" s="9"/>
@@ -6352,20 +6311,20 @@
       <c r="BM20" s="9"/>
       <c r="BN20" s="9"/>
     </row>
-    <row r="21" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="16">
+    <row r="21" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="15">
         <v>22</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="24">
         <v>3658598.1352822352</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="24">
         <v>3701991.4009627872</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="24">
         <v>3736791.2842328846</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="24">
         <v>3778449.7974728658</v>
       </c>
       <c r="F21" s="9"/>
@@ -6428,20 +6387,20 @@
       <c r="BM21" s="9"/>
       <c r="BN21" s="9"/>
     </row>
-    <row r="22" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16">
+    <row r="22" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="15">
         <v>23</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="24">
         <v>3901991.5637460742</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="24">
         <v>3947234.4134572544</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="24">
         <v>3983749.7054528538</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="24">
         <v>4027865.3517051707</v>
       </c>
       <c r="F22" s="9"/>
@@ -6504,20 +6463,20 @@
       <c r="BM22" s="9"/>
       <c r="BN22" s="9"/>
     </row>
-    <row r="23" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="16">
+    <row r="23" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="15">
         <v>24</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="24">
         <v>4153903.7622061465</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="24">
         <v>4201060.9313890282</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="24">
         <v>4239351.6714155218</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="24">
         <v>4286010.450335606</v>
       </c>
       <c r="F23" s="9"/>
@@ -6580,20 +6539,20 @@
       <c r="BM23" s="9"/>
       <c r="BN23" s="9"/>
     </row>
-    <row r="24" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="16">
+    <row r="24" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="15">
         <v>25</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="24">
         <v>4414632.8876123205</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="24">
         <v>4458560.4268118124</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="24">
         <v>4498666.3476713458</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="24">
         <v>4547912.2612623814</v>
       </c>
       <c r="F24" s="9"/>
@@ -6656,20 +6615,20 @@
       <c r="BM24" s="9"/>
       <c r="BN24" s="9"/>
     </row>
-    <row r="25" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="16">
+    <row r="25" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="15">
         <v>26</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="24">
         <v>4684487.5324077122</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="24">
         <v>4730283.3552109972</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="24">
         <v>4772290.3961116606</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="24">
         <v>4824259.0017273193</v>
       </c>
       <c r="F25" s="9"/>
@@ -6732,20 +6691,20 @@
       <c r="BM25" s="9"/>
       <c r="BN25" s="9"/>
     </row>
-    <row r="26" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16">
+    <row r="26" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="15">
         <v>27</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="24">
         <v>4963787.0897709429</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="24">
         <v>5011516.5861041509</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="24">
         <v>5055491.2862473857</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="24">
         <v>5110277.8781085303</v>
       </c>
       <c r="F26" s="9"/>
@@ -6808,20 +6767,20 @@
       <c r="BM26" s="9"/>
       <c r="BN26" s="9"/>
     </row>
-    <row r="27" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16">
+    <row r="27" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="15">
         <v>28</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="24">
         <v>5252862.1316418881</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="24">
         <v>5296815.5059620254</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="24">
         <v>5348604.2075378625</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="24">
         <v>5406307.4151630839</v>
       </c>
       <c r="F27" s="9"/>
@@ -6884,20 +6843,20 @@
       <c r="BM27" s="9"/>
       <c r="BN27" s="9"/>
     </row>
-    <row r="28" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="16">
+    <row r="28" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="15">
         <v>29</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="24">
         <v>5552054.799978314</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="24">
         <v>5597877.3621314662</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="24">
         <v>5651976.0810735049</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="24">
         <v>5712697.9860145459</v>
       </c>
       <c r="F28" s="9"/>
@@ -6960,20 +6919,20 @@
       <c r="BM28" s="9"/>
       <c r="BN28" s="9"/>
     </row>
-    <row r="29" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="16">
+    <row r="29" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="15">
         <v>30</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="24">
         <v>5861719.2117065154</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="24">
         <v>5909476.3832668383</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="24">
         <v>5965965.9701828957</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="24">
         <v>6029812.2268458102</v>
       </c>
       <c r="F29" s="9"/>
@@ -7036,24 +6995,24 @@
       <c r="BM29" s="9"/>
       <c r="BN29" s="9"/>
     </row>
-    <row r="30" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="16">
+    <row r="30" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="15">
         <v>31</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="24">
         <v>6182221.8778452044</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="24">
         <v>6225575.7813165886</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="24">
         <v>6284512.3715812182</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="24">
         <v>6358025.466106168</v>
       </c>
       <c r="F30" s="9"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="16"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
@@ -7112,20 +7071,20 @@
       <c r="BM30" s="9"/>
       <c r="BN30" s="9"/>
     </row>
-    <row r="31" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="16">
+    <row r="31" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="15">
         <v>32</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="24">
         <v>6513942.1372987479</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="24">
         <v>6559144.2471234389</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="24">
         <v>6620641.0308583779</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="24">
         <v>6697726.1687406385</v>
       </c>
       <c r="F31" s="9"/>
@@ -7188,20 +7147,20 @@
       <c r="BM31" s="9"/>
       <c r="BN31" s="9"/>
     </row>
-    <row r="32" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="16">
+    <row r="32" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="15">
         <v>33</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="24">
         <v>6857272.6058331644</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="24">
         <v>6904387.6092335293</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="24">
         <v>6968534.1932102386</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="24">
         <v>7049316.395967315</v>
       </c>
       <c r="F32" s="9"/>
@@ -7264,20 +7223,20 @@
       <c r="BM32" s="9"/>
       <c r="BN32" s="9"/>
     </row>
-    <row r="33" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16">
+    <row r="33" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="15">
         <v>34</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="24">
         <v>7212619.6407662872</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="24">
         <v>7254612.4981869031</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="24">
         <v>7328603.6162444148</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="24">
         <v>7413212.2811469249</v>
       </c>
       <c r="F33" s="9"/>
@@ -7340,20 +7299,20 @@
       <c r="BM33" s="9"/>
       <c r="BN33" s="9"/>
     </row>
-    <row r="34" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="16">
+    <row r="34" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="15">
         <v>35</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="24">
         <v>7580403.8219220685</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="24">
         <v>7624197.2490842156</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="24">
         <v>7701275.4690847863</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="24">
         <v>7789844.5223078225</v>
       </c>
       <c r="F34" s="9"/>
@@ -7416,20 +7375,20 @@
       <c r="BM34" s="9"/>
       <c r="BN34" s="9"/>
     </row>
-    <row r="35" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="16">
+    <row r="35" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="15">
         <v>36</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="24">
         <v>7961060.4494183054</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="24">
         <v>8006717.4662629319</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="24">
         <v>8086990.8367745727</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="24">
         <v>8179658.8919093497</v>
       </c>
       <c r="F35" s="9"/>
@@ -7492,20 +7451,20 @@
       <c r="BM35" s="9"/>
       <c r="BN35" s="9"/>
     </row>
-    <row r="36" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="16">
+    <row r="36" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="15">
         <v>37</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="24">
         <v>8355040.0588769075</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="24">
         <v>8394751.7868609503</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="24">
         <v>8478298.2783080209</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="24">
         <v>8575140.7907870114</v>
       </c>
       <c r="F36" s="9"/>
@@ -7568,20 +7527,20 @@
       <c r="BM36" s="9"/>
       <c r="BN36" s="9"/>
     </row>
-    <row r="37" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="16">
+    <row r="37" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="15">
         <v>38</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="24">
         <v>8762808.9546665624</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="24">
         <v>8804241.4128618501</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="24">
         <v>8891209.4443206191</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="24">
         <v>8992440.529785309</v>
       </c>
       <c r="F37" s="9"/>
@@ -7644,20 +7603,20 @@
       <c r="BM37" s="9"/>
       <c r="BN37" s="9"/>
     </row>
-    <row r="38" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="16">
+    <row r="38" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="15">
         <v>39</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="24">
         <v>9184849.7618088536</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="24">
         <v>9228063.1757727806</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="24">
         <v>9318572.5011436604</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="24">
         <v>9424345.7596485484</v>
       </c>
       <c r="F38" s="9"/>
@@ -7720,20 +7679,20 @@
       <c r="BM38" s="9"/>
       <c r="BN38" s="9"/>
     </row>
-    <row r="39" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="16">
+    <row r="39" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="15">
         <v>40</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="24">
         <v>9621661.9972011242</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="24">
         <v>9657988.5403294638</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="24">
         <v>9760893.2649555095</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="24">
         <v>9871367.6725570001</v>
       </c>
       <c r="F39" s="9"/>
@@ -7796,20 +7755,20 @@
       <c r="BM39" s="9"/>
       <c r="BN39" s="9"/>
     </row>
-    <row r="40" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="16">
+    <row r="40" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="15">
         <v>41</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="24">
         <v>10073762.660832124</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="24">
         <v>10111691.452701762</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="24">
         <v>10218695.255500773</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="24">
         <v>10334035.352417249</v>
       </c>
       <c r="F40" s="9"/>
@@ -7872,20 +7831,20 @@
       <c r="BM40" s="9"/>
       <c r="BN40" s="9"/>
     </row>
-    <row r="41" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16">
+    <row r="41" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="15">
         <v>42</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="24">
         <v>10541686.847690219</v>
       </c>
-      <c r="C41" s="15">
+      <c r="C41" s="24">
         <v>10581273.967007089</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="24">
         <v>10692520.315715119</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="24">
         <v>10812896.401072606</v>
       </c>
       <c r="F41" s="9"/>
@@ -7948,20 +7907,20 @@
       <c r="BM41" s="9"/>
       <c r="BN41" s="9"/>
     </row>
-    <row r="42" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="16">
+    <row r="42" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="15">
         <v>43</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="24">
         <v>11025988.381088352</v>
       </c>
-      <c r="C42" s="15">
+      <c r="C42" s="24">
         <v>11057612.584807269</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="24">
         <v>11173208.346138097</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="24">
         <v>11308517.586430902</v>
       </c>
       <c r="F42" s="9"/>
@@ -8024,20 +7983,20 @@
       <c r="BM42" s="9"/>
       <c r="BN42" s="9"/>
     </row>
-    <row r="43" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="16">
+    <row r="43" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="15">
         <v>44</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="24">
         <v>11527240.468155421</v>
       </c>
-      <c r="C43" s="15">
+      <c r="C43" s="24">
         <v>11560302.33873629</v>
       </c>
-      <c r="D43" s="15">
+      <c r="D43" s="24">
         <v>11680441.364524752</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="24">
         <v>11821485.513276737</v>
       </c>
       <c r="F43" s="9"/>
@@ -8100,20 +8059,20 @@
       <c r="BM43" s="9"/>
       <c r="BN43" s="9"/>
     </row>
-    <row r="44" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="16">
+    <row r="44" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="15">
         <v>45</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="24">
         <v>12046036.378269834</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="24">
         <v>12080586.234052829</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="24">
         <v>12205427.538554937</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="24">
         <v>12352407.317562174</v>
       </c>
       <c r="F44" s="9"/>
@@ -8176,20 +8135,20 @@
       <c r="BM44" s="9"/>
       <c r="BN44" s="9"/>
     </row>
-    <row r="45" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="16">
+    <row r="45" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="15">
         <v>46</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="24">
         <v>12582990.14523826</v>
       </c>
-      <c r="C45" s="15">
+      <c r="C45" s="24">
         <v>12619080.065705447</v>
       </c>
-      <c r="D45" s="15">
+      <c r="D45" s="24">
         <v>12748788.228676178</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="24">
         <v>12901911.384997604</v>
       </c>
       <c r="F45" s="9"/>
@@ -8252,20 +8211,20 @@
       <c r="BM45" s="9"/>
       <c r="BN45" s="9"/>
     </row>
-    <row r="46" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="16">
+    <row r="46" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="15">
         <v>47</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="24">
         <v>13138737.294050574</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="24">
         <v>13176421.181465905</v>
       </c>
-      <c r="D46" s="15">
+      <c r="D46" s="24">
         <v>13311166.542951662</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="24">
         <v>13470648.094793273</v>
       </c>
       <c r="F46" s="9"/>
@@ -8328,20 +8287,20 @@
       <c r="BM46" s="9"/>
       <c r="BN46" s="9"/>
     </row>
-    <row r="47" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="16">
+    <row r="47" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="15">
         <v>48</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="24">
         <v>13713935.593071321</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C47" s="24">
         <v>13753269.236277983</v>
       </c>
-      <c r="D47" s="15">
+      <c r="D47" s="24">
         <v>13893228.098226789</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="24">
         <v>14059290.589431791</v>
       </c>
       <c r="F47" s="9"/>
@@ -8404,20 +8363,20 @@
       <c r="BM47" s="9"/>
       <c r="BN47" s="9"/>
     </row>
-    <row r="48" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="16">
+    <row r="48" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="15">
         <v>49</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="24">
         <v>14309265.832557794</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="24">
         <v>14350306.973008478</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D48" s="24">
         <v>14483712.331354218</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="24">
         <v>14656483.327573342</v>
       </c>
       <c r="F48" s="9"/>
@@ -8480,20 +8439,20 @@
       <c r="BM48" s="9"/>
       <c r="BN48" s="9"/>
     </row>
-    <row r="49" spans="1:66" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="16">
+    <row r="49" spans="1:66" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="15">
         <v>50</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="24">
         <v>14925432.630426297</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="24">
         <v>14968241.030524543</v>
       </c>
-      <c r="D49" s="15">
+      <c r="D49" s="24">
         <v>15106812.989223436</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="24">
         <v>15286630.055359162</v>
       </c>
       <c r="F49" s="9"/>
@@ -8556,7 +8515,7 @@
       <c r="BM49" s="9"/>
       <c r="BN49" s="9"/>
     </row>
-    <row r="50" spans="1:66" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:66" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
@@ -8622,7 +8581,7 @@
       <c r="BM50" s="9"/>
       <c r="BN50" s="9"/>
     </row>
-    <row r="51" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9"/>

</xml_diff>